<commit_message>
REF: Use FRIB/LINAC always.
</commit_message>
<xml_diff>
--- a/phantasy_apps/settings_manager/contrib/templates/template_BDS_20211130T151545.xlsx
+++ b/phantasy_apps/settings_manager/contrib/templates/template_BDS_20211130T151545.xlsx
@@ -83,7 +83,7 @@
     <t xml:space="preserve">segment</t>
   </si>
   <si>
-    <t xml:space="preserve">BDS</t>
+    <t xml:space="preserve">LINAC</t>
   </si>
   <si>
     <t xml:space="preserve">tags</t>
@@ -3019,10 +3019,10 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3166,7 +3166,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>